<commit_message>
updated player displays on home page
</commit_message>
<xml_diff>
--- a/excel layout/New Ideas.xlsx
+++ b/excel layout/New Ideas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Work_application_folder\Github\survivor_game\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Work_application_folder\Github\survivor_game\excel layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F6E351-44D9-481D-AF84-A971DAB4326D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832F19A0-7601-4B7C-B1CA-97F795673746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{9B9077EE-8678-4761-8DF9-84D86FCBDB10}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9B9077EE-8678-4761-8DF9-84D86FCBDB10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="53">
   <si>
     <t>Week 1</t>
   </si>
@@ -139,6 +139,63 @@
   </si>
   <si>
     <t>Eva</t>
+  </si>
+  <si>
+    <t>Jenna</t>
+  </si>
+  <si>
+    <t>Colby</t>
+  </si>
+  <si>
+    <t>Stephanie</t>
+  </si>
+  <si>
+    <t>Cirie</t>
+  </si>
+  <si>
+    <t>Ozzy</t>
+  </si>
+  <si>
+    <t>Coach</t>
+  </si>
+  <si>
+    <t>Aubry</t>
+  </si>
+  <si>
+    <t>Chrissy</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Angelina</t>
+  </si>
+  <si>
+    <t>Mike White</t>
+  </si>
+  <si>
+    <t>Rick</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Dee</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>Tiffany</t>
+  </si>
+  <si>
+    <t>Genevieve</t>
   </si>
 </sst>
 </file>
@@ -215,7 +272,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -238,13 +295,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -253,13 +321,16 @@
     <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -599,7 +670,7 @@
   <dimension ref="A1:V41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+      <selection activeCell="Y26" sqref="Y26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,26 +683,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
@@ -958,26 +1029,26 @@
       </c>
     </row>
     <row r="8" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
       <c r="U8" t="s">
         <v>27</v>
       </c>
@@ -1038,15 +1109,15 @@
       <c r="R9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="9" t="s">
+      <c r="T9" s="8" t="s">
         <v>29</v>
       </c>
       <c r="U9">
-        <v>107</v>
-      </c>
-      <c r="V9" s="10">
-        <f>MIN(92.44+(4*(U9/$U$14) - 1)*92.44, 184.88)</f>
-        <v>149.86484848484847</v>
+        <v>10</v>
+      </c>
+      <c r="V9" s="9">
+        <f>MIN(5+(22*(U9/$U$31) - 1)*5, 10)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1120,15 +1191,15 @@
         <f t="shared" ref="R10" si="17">R11*2</f>
         <v>184.88425889503631</v>
       </c>
-      <c r="T10" s="9" t="s">
+      <c r="T10" s="8" t="s">
         <v>30</v>
       </c>
       <c r="U10">
-        <v>67</v>
-      </c>
-      <c r="V10" s="10">
-        <f t="shared" ref="V10:V13" si="18">MIN(92.44+(4*(U10/$U$14) - 1)*92.44, 184.88)</f>
-        <v>93.840606060606063</v>
+        <v>10</v>
+      </c>
+      <c r="V10" s="9">
+        <f t="shared" ref="V10:V30" si="18">MIN(5+(22*(U10/$U$31) - 1)*5, 10)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1202,15 +1273,15 @@
         <f t="shared" si="19"/>
         <v>92.442129447518155</v>
       </c>
-      <c r="T11" s="9" t="s">
+      <c r="T11" s="8" t="s">
         <v>31</v>
       </c>
       <c r="U11">
-        <v>75</v>
-      </c>
-      <c r="V11" s="10">
+        <v>10</v>
+      </c>
+      <c r="V11" s="9">
         <f t="shared" si="18"/>
-        <v>105.04545454545455</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1268,15 +1339,15 @@
       <c r="R12" s="5">
         <v>0.01</v>
       </c>
-      <c r="T12" s="9" t="s">
-        <v>32</v>
+      <c r="T12" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="U12">
-        <v>1</v>
-      </c>
-      <c r="V12" s="10">
+        <v>10</v>
+      </c>
+      <c r="V12" s="9">
         <f t="shared" si="18"/>
-        <v>1.4006060606060657</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1332,52 +1403,62 @@
       <c r="R13" s="6">
         <v>0.2</v>
       </c>
-      <c r="T13" s="9" t="s">
-        <v>33</v>
+      <c r="T13" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="U13">
-        <v>14</v>
-      </c>
-      <c r="V13" s="10">
+        <v>10</v>
+      </c>
+      <c r="V13" s="9">
         <f t="shared" si="18"/>
-        <v>19.608484848484849</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="T14" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="U14">
-        <f>SUM(U9:U13)</f>
-        <v>264</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="V14" s="9">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="U15" t="s">
-        <v>27</v>
-      </c>
-      <c r="V15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="T15" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="U15">
+        <v>10</v>
+      </c>
+      <c r="V15" s="9">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
         <v>0</v>
@@ -1430,18 +1511,18 @@
       <c r="R16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="T16" s="9" t="s">
-        <v>29</v>
+      <c r="T16" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="U16">
-        <v>107</v>
-      </c>
-      <c r="V16" s="10">
-        <f>MIN(92.44+(4*(U16/$U$14) - 1)*92.44, 184.88)</f>
-        <v>149.86484848484847</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="V16" s="9">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1512,18 +1593,18 @@
         <f t="shared" si="20"/>
         <v>93.57620873536672</v>
       </c>
-      <c r="T17" s="9" t="s">
-        <v>30</v>
+      <c r="T17" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="U17">
-        <v>67</v>
-      </c>
-      <c r="V17" s="10">
-        <f t="shared" ref="V17:V20" si="21">MIN(92.44+(4*(U17/$U$14) - 1)*92.44, 184.88)</f>
-        <v>93.840606060606063</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="V17" s="9">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -1535,77 +1616,77 @@
         <v>5.75</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" ref="D18:R18" si="22">C18*(1.15)</f>
+        <f t="shared" ref="D18:R18" si="21">C18*(1.15)</f>
         <v>6.6124999999999998</v>
       </c>
       <c r="E18" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>7.6043749999999992</v>
       </c>
       <c r="F18" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>8.7450312499999985</v>
       </c>
       <c r="G18" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>10.056785937499997</v>
       </c>
       <c r="H18" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>11.565303828124996</v>
       </c>
       <c r="I18" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>13.300099402343745</v>
       </c>
       <c r="J18" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>15.295114312695306</v>
       </c>
       <c r="K18" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>17.589381459599601</v>
       </c>
       <c r="L18" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>20.22778867853954</v>
       </c>
       <c r="M18" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>23.26195698032047</v>
       </c>
       <c r="N18" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>26.751250527368537</v>
       </c>
       <c r="O18" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>30.763938106473816</v>
       </c>
       <c r="P18" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>35.378528822444885</v>
       </c>
       <c r="Q18" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>40.685308145811618</v>
       </c>
       <c r="R18" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>46.78810436768336</v>
       </c>
-      <c r="T18" s="9" t="s">
-        <v>31</v>
+      <c r="T18" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="U18">
-        <v>75</v>
-      </c>
-      <c r="V18" s="10">
-        <f t="shared" si="21"/>
-        <v>105.04545454545455</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="V18" s="9">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -1660,18 +1741,18 @@
       <c r="R19" s="5">
         <v>0.01</v>
       </c>
-      <c r="T19" s="9" t="s">
-        <v>32</v>
+      <c r="T19" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="U19">
-        <v>1</v>
-      </c>
-      <c r="V19" s="10">
-        <f t="shared" si="21"/>
-        <v>1.4006060606060657</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="V19" s="9">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -1724,44 +1805,60 @@
       <c r="R20" s="6">
         <v>0.15</v>
       </c>
-      <c r="T20" s="9" t="s">
-        <v>33</v>
+      <c r="T20" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="U20">
-        <v>14</v>
-      </c>
-      <c r="V20" s="10">
-        <f t="shared" si="21"/>
-        <v>19.608484848484849</v>
+        <v>10</v>
+      </c>
+      <c r="V20" s="9">
+        <f t="shared" si="18"/>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="T21" s="11" t="s">
+        <v>43</v>
+      </c>
       <c r="U21">
-        <f>SUM(U16:U20)</f>
-        <v>264</v>
+        <v>10</v>
+      </c>
+      <c r="V21" s="9">
+        <f t="shared" si="18"/>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="T22" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="U22">
+        <v>10</v>
+      </c>
+      <c r="V22" s="9">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
@@ -1816,6 +1913,16 @@
       <c r="R23" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="T23" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="U23">
+        <v>10</v>
+      </c>
+      <c r="V23" s="9">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
@@ -1829,64 +1936,74 @@
         <v>11</v>
       </c>
       <c r="D24" s="5">
-        <f t="shared" ref="D24:R24" si="23">D25*2</f>
+        <f t="shared" ref="D24:R24" si="22">D25*2</f>
         <v>12.100000000000001</v>
       </c>
       <c r="E24" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>13.310000000000002</v>
       </c>
       <c r="F24" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>14.641000000000004</v>
       </c>
       <c r="G24" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>16.105100000000004</v>
       </c>
       <c r="H24" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>17.715610000000005</v>
       </c>
       <c r="I24" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>19.487171000000007</v>
       </c>
       <c r="J24" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>21.43588810000001</v>
       </c>
       <c r="K24" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>23.579476910000015</v>
       </c>
       <c r="L24" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>25.937424601000018</v>
       </c>
       <c r="M24" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>28.531167061100021</v>
       </c>
       <c r="N24" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>31.384283767210025</v>
       </c>
       <c r="O24" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>34.522712143931031</v>
       </c>
       <c r="P24" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>37.974983358324138</v>
       </c>
       <c r="Q24" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>41.772481694156554</v>
       </c>
       <c r="R24" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>45.949729863572216</v>
+      </c>
+      <c r="T24" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="U24">
+        <v>10</v>
+      </c>
+      <c r="V24" s="9">
+        <f t="shared" si="18"/>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
@@ -1901,64 +2018,74 @@
         <v>5.5</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" ref="D25:R25" si="24">C25*(1.1)</f>
+        <f t="shared" ref="D25:R25" si="23">C25*(1.1)</f>
         <v>6.0500000000000007</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>6.6550000000000011</v>
       </c>
       <c r="F25" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>7.3205000000000018</v>
       </c>
       <c r="G25" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>8.0525500000000019</v>
       </c>
       <c r="H25" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>8.8578050000000026</v>
       </c>
       <c r="I25" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>9.7435855000000036</v>
       </c>
       <c r="J25" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>10.717944050000005</v>
       </c>
       <c r="K25" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>11.789738455000007</v>
       </c>
       <c r="L25" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>12.968712300500009</v>
       </c>
       <c r="M25" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>14.26558353055001</v>
       </c>
       <c r="N25" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>15.692141883605013</v>
       </c>
       <c r="O25" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>17.261356071965515</v>
       </c>
       <c r="P25" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>18.987491679162069</v>
       </c>
       <c r="Q25" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>20.886240847078277</v>
       </c>
       <c r="R25" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>22.974864931786108</v>
+      </c>
+      <c r="T25" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="U25">
+        <v>10</v>
+      </c>
+      <c r="V25" s="9">
+        <f t="shared" si="18"/>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
@@ -2016,6 +2143,16 @@
       <c r="R26" s="5">
         <v>0.01</v>
       </c>
+      <c r="T26" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="U26">
+        <v>10</v>
+      </c>
+      <c r="V26" s="9">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
@@ -2070,28 +2207,60 @@
       <c r="R27" s="6">
         <v>0.1</v>
       </c>
+      <c r="T27" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="U27">
+        <v>10</v>
+      </c>
+      <c r="V27" s="9">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="T28" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="U28">
+        <v>10</v>
+      </c>
+      <c r="V28" s="9">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="T29" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="U29">
+        <v>10</v>
+      </c>
+      <c r="V29" s="9">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
@@ -2146,6 +2315,16 @@
       <c r="R30" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="T30" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="U30">
+        <v>10</v>
+      </c>
+      <c r="V30" s="9">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
@@ -2159,64 +2338,69 @@
         <v>10.5</v>
       </c>
       <c r="D31" s="5">
-        <f t="shared" ref="D31:R31" si="25">D32*2</f>
+        <f t="shared" ref="D31:R31" si="24">D32*2</f>
         <v>11.025</v>
       </c>
       <c r="E31" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>11.576250000000002</v>
       </c>
       <c r="F31" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>12.155062500000001</v>
       </c>
       <c r="G31" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>12.762815625000002</v>
       </c>
       <c r="H31" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>13.400956406250003</v>
       </c>
       <c r="I31" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>14.071004226562504</v>
       </c>
       <c r="J31" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>14.774554437890631</v>
       </c>
       <c r="K31" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>15.513282159785163</v>
       </c>
       <c r="L31" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>16.288946267774421</v>
       </c>
       <c r="M31" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>17.103393581163143</v>
       </c>
       <c r="N31" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>17.9585632602213</v>
       </c>
       <c r="O31" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>18.856491423232367</v>
       </c>
       <c r="P31" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>19.799315994393986</v>
       </c>
       <c r="Q31" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>20.789281794113688</v>
       </c>
       <c r="R31" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>21.828745883819373</v>
+      </c>
+      <c r="T31" s="11"/>
+      <c r="U31">
+        <f>SUM(U9:U30)</f>
+        <v>220</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.3">
@@ -2231,65 +2415,66 @@
         <v>5.25</v>
       </c>
       <c r="D32" s="4">
-        <f t="shared" ref="D32:R32" si="26">C32*(1.05)</f>
+        <f t="shared" ref="D32:R32" si="25">C32*(1.05)</f>
         <v>5.5125000000000002</v>
       </c>
       <c r="E32" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>5.7881250000000009</v>
       </c>
       <c r="F32" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>6.0775312500000007</v>
       </c>
       <c r="G32" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>6.3814078125000009</v>
       </c>
       <c r="H32" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>6.7004782031250016</v>
       </c>
       <c r="I32" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>7.0355021132812521</v>
       </c>
       <c r="J32" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>7.3872772189453153</v>
       </c>
       <c r="K32" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>7.7566410798925816</v>
       </c>
       <c r="L32" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>8.1444731338872103</v>
       </c>
       <c r="M32" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>8.5516967905815715</v>
       </c>
       <c r="N32" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>8.9792816301106502</v>
       </c>
       <c r="O32" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>9.4282457116161833</v>
       </c>
       <c r="P32" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>9.8996579971969929</v>
       </c>
       <c r="Q32" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>10.394640897056844</v>
       </c>
       <c r="R32" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>10.914372941909686</v>
       </c>
+      <c r="T32" s="11"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
@@ -2402,26 +2587,26 @@
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
@@ -2489,63 +2674,63 @@
         <v>10.1</v>
       </c>
       <c r="D38" s="5">
-        <f t="shared" ref="D38:R38" si="27">D39*2</f>
+        <f t="shared" ref="D38:R38" si="26">D39*2</f>
         <v>10.201000000000001</v>
       </c>
       <c r="E38" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>10.30301</v>
       </c>
       <c r="F38" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>10.4060401</v>
       </c>
       <c r="G38" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>10.510100501</v>
       </c>
       <c r="H38" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>10.615201506010001</v>
       </c>
       <c r="I38" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>10.721353521070101</v>
       </c>
       <c r="J38" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>10.828567056280802</v>
       </c>
       <c r="K38" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>10.936852726843609</v>
       </c>
       <c r="L38" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>11.046221254112046</v>
       </c>
       <c r="M38" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>11.156683466653167</v>
       </c>
       <c r="N38" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>11.268250301319698</v>
       </c>
       <c r="O38" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>11.380932804332895</v>
       </c>
       <c r="P38" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>11.494742132376224</v>
       </c>
       <c r="Q38" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>11.609689553699987</v>
       </c>
       <c r="R38" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>11.725786449236987</v>
       </c>
     </row>
@@ -2561,63 +2746,63 @@
         <v>5.05</v>
       </c>
       <c r="D39" s="4">
-        <f t="shared" ref="D39:R39" si="28">C39*(1.01)</f>
+        <f t="shared" ref="D39:R39" si="27">C39*(1.01)</f>
         <v>5.1005000000000003</v>
       </c>
       <c r="E39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>5.1515050000000002</v>
       </c>
       <c r="F39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>5.2030200500000001</v>
       </c>
       <c r="G39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>5.2550502505000001</v>
       </c>
       <c r="H39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>5.3076007530050004</v>
       </c>
       <c r="I39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>5.3606767605350507</v>
       </c>
       <c r="J39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>5.4142835281404009</v>
       </c>
       <c r="K39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>5.4684263634218047</v>
       </c>
       <c r="L39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>5.5231106270560231</v>
       </c>
       <c r="M39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>5.5783417333265835</v>
       </c>
       <c r="N39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>5.6341251506598491</v>
       </c>
       <c r="O39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>5.6904664021664475</v>
       </c>
       <c r="P39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>5.7473710661881121</v>
       </c>
       <c r="Q39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>5.8048447768499933</v>
       </c>
       <c r="R39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>5.8628932246184933</v>
       </c>
     </row>
@@ -2750,7 +2935,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2764,61 +2949,61 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B2">
         <v>107</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="9">
         <f>MIN(92.44+(4*(B2/$B$7) - 1)*92.44, 184.88)</f>
         <v>149.86484848484847</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B3">
         <v>67</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <f t="shared" ref="C3:C6" si="0">MIN(92.44+(4*(B3/$B$7) - 1)*92.44, 184.88)</f>
         <v>93.840606060606063</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B4">
         <v>75</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <f t="shared" si="0"/>
         <v>105.04545454545455</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <f t="shared" si="0"/>
         <v>1.4006060606060657</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B6">
         <v>14</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <f t="shared" si="0"/>
         <v>19.608484848484849</v>
       </c>

</xml_diff>